<commit_message>
Added merge conflicts commands
</commit_message>
<xml_diff>
--- a/GitCheatSheet.xlsx
+++ b/GitCheatSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>git status</t>
   </si>
@@ -160,6 +160,36 @@
   </si>
   <si>
     <t>Set core.editor to vim</t>
+  </si>
+  <si>
+    <t>git branch -v</t>
+  </si>
+  <si>
+    <t>This shows names of branch with their commit hash and commit message</t>
+  </si>
+  <si>
+    <t>git branch --merged</t>
+  </si>
+  <si>
+    <t>git branch --no-merged</t>
+  </si>
+  <si>
+    <t>Already merged branches</t>
+  </si>
+  <si>
+    <t>Not already merged branches</t>
+  </si>
+  <si>
+    <t>git branch -d develop</t>
+  </si>
+  <si>
+    <t>Gives error if develop is not merged</t>
+  </si>
+  <si>
+    <t>git branch -D develop</t>
+  </si>
+  <si>
+    <t>No error and branch gets deleted</t>
   </si>
 </sst>
 </file>
@@ -486,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G28"/>
+  <dimension ref="C3:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,6 +809,61 @@
         <v>46</v>
       </c>
     </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E29" s="1">
+        <v>27</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E30" s="1">
+        <v>28</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E31" s="1">
+        <v>29</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E32" s="1">
+        <v>30</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="1">
+        <v>31</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added commands for pushing new branches to github
</commit_message>
<xml_diff>
--- a/GitCheatSheet.xlsx
+++ b/GitCheatSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>git status</t>
   </si>
@@ -189,7 +189,19 @@
     <t>git branch -D develop</t>
   </si>
   <si>
-    <t xml:space="preserve">No error and branch gets </t>
+    <t>No error and branch gets deleted</t>
+  </si>
+  <si>
+    <t>git branch -d origin develop</t>
+  </si>
+  <si>
+    <t>git push origin develop</t>
+  </si>
+  <si>
+    <t>Deletes develop branch from github website</t>
+  </si>
+  <si>
+    <t>pushes develop branch to github</t>
   </si>
 </sst>
 </file>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G33"/>
+  <dimension ref="C3:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,6 +876,28 @@
         <v>56</v>
       </c>
     </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" s="1">
+        <v>32</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="1">
+        <v>33</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>